<commit_message>
Update all city code
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\Traveloka_DataAutomation_Performer_API\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388B4852-9586-4401-A04C-BAD9DA0E2E12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AC0B94-BB90-408E-8F9F-FB1842E71A59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="91">
   <si>
     <t>Name</t>
   </si>
@@ -250,6 +250,54 @@
   </si>
   <si>
     <t>Endpoint</t>
+  </si>
+  <si>
+    <t>RPA180_WSAP</t>
+  </si>
+  <si>
+    <t>RPA181_OfficeID1</t>
+  </si>
+  <si>
+    <t>RPA182_OfficeID1</t>
+  </si>
+  <si>
+    <t>RPA183_OfficeID1</t>
+  </si>
+  <si>
+    <t>RPA183_WSAP</t>
+  </si>
+  <si>
+    <t>RPA180_OfficeID1</t>
+  </si>
+  <si>
+    <t>RPA180_Amadeus_TJQ_TH_OfficeID1</t>
+  </si>
+  <si>
+    <t>BKKIQ317O</t>
+  </si>
+  <si>
+    <t>RPA181_Amadeus_TJQ_VN_OfficeID1</t>
+  </si>
+  <si>
+    <t>SGNTV2001</t>
+  </si>
+  <si>
+    <t>RPA182_Amadeus_TJQ_SG_OfficeID1</t>
+  </si>
+  <si>
+    <t>SINTV2100</t>
+  </si>
+  <si>
+    <t>RPA183_Amadeus_TJQ_MY_OfficeID1</t>
+  </si>
+  <si>
+    <t>KULTV28AA</t>
+  </si>
+  <si>
+    <t>RPA181_WSAP</t>
+  </si>
+  <si>
+    <t>RPA182_WSAP</t>
   </si>
 </sst>
 </file>
@@ -2907,10 +2955,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z995"/>
+  <dimension ref="A1:Z991"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3044,50 +3092,98 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="D12" s="2"/>
+      <c r="A12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" t="s">
+        <v>68</v>
+      </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="D14" s="2"/>
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="D16" s="2"/>
+      <c r="A16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>86</v>
+      </c>
     </row>
-    <row r="17" spans="4:4" ht="14.25" customHeight="1">
+    <row r="17" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" t="s">
+        <v>68</v>
+      </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="4:4" ht="14.25" customHeight="1">
-      <c r="D18" s="2"/>
+    <row r="18" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>88</v>
+      </c>
     </row>
-    <row r="19" spans="4:4" ht="14.25" customHeight="1">
+    <row r="19" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" t="s">
+        <v>68</v>
+      </c>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="4:4" ht="14.25" customHeight="1">
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="4:4" ht="14.25" customHeight="1">
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="4:4" ht="14.25" customHeight="1">
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="4:4" ht="14.25" customHeight="1">
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="4:4" ht="14.25" customHeight="1"/>
-    <row r="25" spans="4:4" ht="14.25" customHeight="1"/>
-    <row r="26" spans="4:4" ht="14.25" customHeight="1"/>
-    <row r="27" spans="4:4" ht="14.25" customHeight="1"/>
-    <row r="28" spans="4:4" ht="14.25" customHeight="1"/>
-    <row r="29" spans="4:4" ht="14.25" customHeight="1"/>
-    <row r="30" spans="4:4" ht="14.25" customHeight="1"/>
-    <row r="31" spans="4:4" ht="14.25" customHeight="1"/>
-    <row r="32" spans="4:4" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -4047,10 +4143,6 @@
     <row r="989" ht="14.25" customHeight="1"/>
     <row r="990" ht="14.25" customHeight="1"/>
     <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update test pre SIT
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\Traveloka_DataAutomation_Performer_API\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AC0B94-BB90-408E-8F9F-FB1842E71A59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68AA134C-5A5E-4A55-B43D-95A7EBC93DBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="99">
   <si>
     <t>Name</t>
   </si>
@@ -298,6 +298,30 @@
   </si>
   <si>
     <t>RPA182_WSAP</t>
+  </si>
+  <si>
+    <t>RPA180_OfficeID2</t>
+  </si>
+  <si>
+    <t>RPA180_Amadeus_TJQ_TH_OfficeID2</t>
+  </si>
+  <si>
+    <t>RPA180_OfficeID3</t>
+  </si>
+  <si>
+    <t>RPA180_Amadeus_TJQ_TH_OfficeID3</t>
+  </si>
+  <si>
+    <t>RPA180_OfficeID4</t>
+  </si>
+  <si>
+    <t>RPA180_Amadeus_TJQ_TH_OfficeID4</t>
+  </si>
+  <si>
+    <t>RPA183_OfficeID2</t>
+  </si>
+  <si>
+    <t>RPA183_Amadeus_TJQ_MY_OfficeID2</t>
   </si>
 </sst>
 </file>
@@ -2955,10 +2979,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z991"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3104,77 +3128,109 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="B14" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>84</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>86</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="2"/>
+        <v>83</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>88</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1">
       <c r="A19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
         <v>79</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B23" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:4" ht="14.25" customHeight="1"/>
+      <c r="D23" s="2"/>
+    </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:4" ht="14.25" customHeight="1"/>
@@ -4143,6 +4199,10 @@
     <row r="989" ht="14.25" customHeight="1"/>
     <row r="990" ht="14.25" customHeight="1"/>
     <row r="991" ht="14.25" customHeight="1"/>
+    <row r="992" ht="14.25" customHeight="1"/>
+    <row r="993" ht="14.25" customHeight="1"/>
+    <row r="994" ht="14.25" customHeight="1"/>
+    <row r="995" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>